<commit_message>
Update schedule file: Y4_B2526_General_&_Special_surgery_1_B1_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_Special_surgery_1_B1_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_Special_surgery_1_B1_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1462,6 +1462,1896 @@
         <v>180</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>186</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>23/11/2024</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>187</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>24/11/2024</t>
+        </is>
+      </c>
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>25/11/2024</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>30/11/2024</t>
+        </is>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>01/12/2024</t>
+        </is>
+      </c>
+      <c r="F33" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G33" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>191</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>02/12/2024</t>
+        </is>
+      </c>
+      <c r="F34" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="inlineStr">
+        <is>
+          <t>192</t>
+        </is>
+      </c>
+      <c r="E35" s="7" t="inlineStr">
+        <is>
+          <t>07/12/2024</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>193</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>08/12/2024</t>
+        </is>
+      </c>
+      <c r="F36" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>194</t>
+        </is>
+      </c>
+      <c r="E37" s="7" t="inlineStr">
+        <is>
+          <t>09/12/2024</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G37" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>14/12/2024</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>196</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>15/12/2024</t>
+        </is>
+      </c>
+      <c r="F39" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G39" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>197</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>16/12/2024</t>
+        </is>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>198</t>
+        </is>
+      </c>
+      <c r="E41" s="7" t="inlineStr">
+        <is>
+          <t>21/12/2024</t>
+        </is>
+      </c>
+      <c r="F41" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>199</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>22/12/2024</t>
+        </is>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D43" s="6" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E43" s="7" t="inlineStr">
+        <is>
+          <t>23/12/2024</t>
+        </is>
+      </c>
+      <c r="F43" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G43" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>28/12/2024</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>202</t>
+        </is>
+      </c>
+      <c r="E45" s="7" t="inlineStr">
+        <is>
+          <t>29/12/2024</t>
+        </is>
+      </c>
+      <c r="F45" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G45" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>30/12/2024</t>
+        </is>
+      </c>
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>204</t>
+        </is>
+      </c>
+      <c r="E47" s="7" t="inlineStr">
+        <is>
+          <t>04/01/2025</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>205</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>05/01/2025</t>
+        </is>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>206</t>
+        </is>
+      </c>
+      <c r="E49" s="7" t="inlineStr">
+        <is>
+          <t>06/01/2025</t>
+        </is>
+      </c>
+      <c r="F49" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>207</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>11/01/2025</t>
+        </is>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>208</t>
+        </is>
+      </c>
+      <c r="E51" s="7" t="inlineStr">
+        <is>
+          <t>12/01/2025</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G51" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>209</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>13/01/2025</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>210</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
+          <t>18/01/2025</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>211</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>19/01/2025</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B55" s="6" t="inlineStr">
+        <is>
+          <t>B1B</t>
+        </is>
+      </c>
+      <c r="C55" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>212</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>20/01/2025</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C57" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E57" s="7" t="inlineStr">
+        <is>
+          <t>23/11/2025</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>24/11/2025</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E59" s="7" t="inlineStr">
+        <is>
+          <t>29/11/2025</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
+        <is>
+          <t>30/11/2025</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E61" s="7" t="inlineStr">
+        <is>
+          <t>01/12/2025</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>06/12/2025</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
+          <t>07/12/2025</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>08/12/2025</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E65" s="7" t="inlineStr">
+        <is>
+          <t>13/12/2025</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E66" s="3" t="inlineStr">
+        <is>
+          <t>14/12/2025</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B67" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E67" s="7" t="inlineStr">
+        <is>
+          <t>15/12/2025</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>20/12/2025</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E69" s="7" t="inlineStr">
+        <is>
+          <t>21/12/2025</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>22/12/2025</t>
+        </is>
+      </c>
+      <c r="F70" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E71" s="7" t="inlineStr">
+        <is>
+          <t>27/12/2025</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>28/12/2025</t>
+        </is>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E73" s="7" t="inlineStr">
+        <is>
+          <t>29/12/2025</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G73" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>03/01/2026</t>
+        </is>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E75" s="7" t="inlineStr">
+        <is>
+          <t>04/01/2026</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>05/01/2026</t>
+        </is>
+      </c>
+      <c r="F76" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E77" s="7" t="inlineStr">
+        <is>
+          <t>10/01/2026</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="inlineStr">
+        <is>
+          <t>11/01/2026</t>
+        </is>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="E79" s="7" t="inlineStr">
+        <is>
+          <t>12/01/2026</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>17/01/2026</t>
+        </is>
+      </c>
+      <c r="F80" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E81" s="7" t="inlineStr">
+        <is>
+          <t>18/01/2026</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>B1C</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>clinical</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>19/01/2026</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>